<commit_message>
Comienza la actualización de partidos, grupos A y B
</commit_message>
<xml_diff>
--- a/docs/fifa-world-cup-2022-UTC_excel.xlsx
+++ b/docs/fifa-world-cup-2022-UTC_excel.xlsx
@@ -1,31 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Documents/PROYECTOS/02.CURSO_HTML/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A6B9360D-2F98-AD46-A50F-66FCA3F04602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9547178-0F85-F34F-9492-4877CA9EF5A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="12280" windowHeight="17040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fifa-world-cup-2022-UTC_excel" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'fifa-world-cup-2022-UTC_excel'!$A$1:$H$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Hoja1!$C$1:$C$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'fifa-world-cup-2022-UTC_excel'!$A$1:$I$65</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Hoja1!$C$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="89">
   <si>
     <t>Match Number</t>
   </si>
@@ -262,12 +262,42 @@
   </si>
   <si>
     <t>list of countries</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>POSICION</t>
+  </si>
+  <si>
+    <t>match_db</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>B4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1102,19 +1132,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H65"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1122,1451 +1153,1495 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
         <v>44886.666666666664</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>18</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1">
         <v>44886.416666666664</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>9</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>10</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1">
         <v>44886.541666666664</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>13</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>14</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1">
         <v>44886.791666666664</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>19</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>20</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>21</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="1">
         <v>44887.791666666664</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>33</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>34</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>35</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D7" s="1">
         <v>44887.541666666664</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>26</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>27</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>28</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
-      <c r="C8" s="1">
+      <c r="D8" s="1">
         <v>44887.666666666664</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>30</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>31</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>32</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
-      <c r="C9" s="1">
+      <c r="D9" s="1">
         <v>44887.416666666664</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>22</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>23</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>24</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10" s="1">
+      <c r="D10" s="1">
         <v>44888.791666666664</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>19</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>44</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>45</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
-      <c r="C11" s="1">
+      <c r="D11" s="1">
         <v>44888.666666666664</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>8</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>42</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>43</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
-      <c r="C12" s="1">
+      <c r="D12" s="1">
         <v>44888.541666666664</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>12</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>39</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>40</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
-      <c r="C13" s="1">
+      <c r="D13" s="1">
         <v>44888.416666666664</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>16</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>36</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>37</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
-      <c r="C14" s="1">
+      <c r="D14" s="1">
         <v>44889.416666666664</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>33</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>46</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>47</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
-      <c r="C15" s="1">
+      <c r="D15" s="1">
         <v>44889.541666666664</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>26</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>49</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>50</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
-      <c r="C16" s="1">
+      <c r="D16" s="1">
         <v>44889.666666666664</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>30</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>52</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>53</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
-      <c r="C17" s="1">
+      <c r="D17" s="1">
         <v>44889.791666666664</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>22</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>54</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>55</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18">
         <v>2</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18">
+        <v>9</v>
+      </c>
+      <c r="D18" s="1">
         <v>44890.416666666664</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>19</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>21</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>14</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19">
         <v>2</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19" s="1">
         <v>44890.541666666664</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>8</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>17</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>9</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20">
         <v>2</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20" s="1">
         <v>44890.666666666664</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>12</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>10</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>18</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21">
         <v>2</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21">
+        <v>10</v>
+      </c>
+      <c r="D21" s="1">
         <v>44890.791666666664</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>16</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>13</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>20</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22">
         <v>2</v>
       </c>
-      <c r="C22" s="1">
+      <c r="D22" s="1">
         <v>44891.416666666664</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>33</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>28</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>35</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23">
         <v>2</v>
       </c>
-      <c r="C23" s="1">
+      <c r="D23" s="1">
         <v>44891.541666666664</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>26</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>32</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>24</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24">
         <v>2</v>
       </c>
-      <c r="C24" s="1">
+      <c r="D24" s="1">
         <v>44891.666666666664</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>30</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>34</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>27</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25">
         <v>2</v>
       </c>
-      <c r="C25" s="1">
+      <c r="D25" s="1">
         <v>44891.791666666664</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>22</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>23</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>31</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26">
         <v>2</v>
       </c>
-      <c r="C26" s="1">
+      <c r="D26" s="1">
         <v>44892.416666666664</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>19</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>40</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>43</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27">
         <v>2</v>
       </c>
-      <c r="C27" s="1">
+      <c r="D27" s="1">
         <v>44892.541666666664</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>8</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>44</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>36</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28">
         <v>2</v>
       </c>
-      <c r="C28" s="1">
+      <c r="D28" s="1">
         <v>44892.666666666664</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>12</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>37</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>45</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29">
         <v>2</v>
       </c>
-      <c r="C29" s="1">
+      <c r="D29" s="1">
         <v>44892.791666666664</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>16</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>42</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>39</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30">
         <v>2</v>
       </c>
-      <c r="C30" s="1">
+      <c r="D30" s="1">
         <v>44893.416666666664</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>33</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>47</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>55</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31">
         <v>2</v>
       </c>
-      <c r="C31" s="1">
+      <c r="D31" s="1">
         <v>44893.541666666664</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>26</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>50</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>53</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32">
         <v>2</v>
       </c>
-      <c r="C32" s="1">
+      <c r="D32" s="1">
         <v>44893.666666666664</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>30</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>54</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>46</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33">
         <v>2</v>
       </c>
-      <c r="C33" s="1">
+      <c r="D33" s="1">
         <v>44893.791666666664</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>22</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>52</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>49</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34">
         <v>3</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C34">
+        <v>11</v>
+      </c>
+      <c r="D34" s="1">
         <v>44894.791666666664</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>19</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>21</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>13</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35">
         <v>3</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35">
+        <v>12</v>
+      </c>
+      <c r="D35" s="1">
         <v>44894.791666666664</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>8</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>14</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>20</v>
       </c>
-      <c r="G35" t="s">
+      <c r="H35" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36">
         <v>3</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36">
+        <v>5</v>
+      </c>
+      <c r="D36" s="1">
         <v>44894.625</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>12</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>18</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>9</v>
       </c>
-      <c r="G36" t="s">
+      <c r="H36" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37">
         <v>3</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C37">
+        <v>6</v>
+      </c>
+      <c r="D37" s="1">
         <v>44894.625</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>16</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>10</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>17</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38">
         <v>3</v>
       </c>
-      <c r="C38" s="1">
+      <c r="D38" s="1">
         <v>44895.625</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>33</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" t="s">
         <v>35</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G38" t="s">
         <v>27</v>
       </c>
-      <c r="G38" t="s">
+      <c r="H38" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39">
         <v>3</v>
       </c>
-      <c r="C39" s="1">
+      <c r="D39" s="1">
         <v>44895.625</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>26</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F39" t="s">
         <v>28</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>34</v>
       </c>
-      <c r="G39" t="s">
+      <c r="H39" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40">
         <v>3</v>
       </c>
-      <c r="C40" s="1">
+      <c r="D40" s="1">
         <v>44895.791666666664</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>30</v>
       </c>
-      <c r="E40" t="s">
+      <c r="F40" t="s">
         <v>32</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>23</v>
       </c>
-      <c r="G40" t="s">
+      <c r="H40" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41">
         <v>3</v>
       </c>
-      <c r="C41" s="1">
+      <c r="D41" s="1">
         <v>44895.791666666664</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>22</v>
       </c>
-      <c r="E41" t="s">
+      <c r="F41" t="s">
         <v>24</v>
       </c>
-      <c r="F41" t="s">
+      <c r="G41" t="s">
         <v>31</v>
       </c>
-      <c r="G41" t="s">
+      <c r="H41" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42">
         <v>3</v>
       </c>
-      <c r="C42" s="1">
+      <c r="D42" s="1">
         <v>44896.625</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>19</v>
       </c>
-      <c r="E42" t="s">
+      <c r="F42" t="s">
         <v>37</v>
       </c>
-      <c r="F42" t="s">
+      <c r="G42" t="s">
         <v>44</v>
       </c>
-      <c r="G42" t="s">
+      <c r="H42" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43">
         <v>3</v>
       </c>
-      <c r="C43" s="1">
+      <c r="D43" s="1">
         <v>44896.625</v>
       </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
         <v>8</v>
       </c>
-      <c r="E43" t="s">
+      <c r="F43" t="s">
         <v>45</v>
       </c>
-      <c r="F43" t="s">
+      <c r="G43" t="s">
         <v>36</v>
       </c>
-      <c r="G43" t="s">
+      <c r="H43" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44">
         <v>3</v>
       </c>
-      <c r="C44" s="1">
+      <c r="D44" s="1">
         <v>44896.791666666664</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
         <v>12</v>
       </c>
-      <c r="E44" t="s">
+      <c r="F44" t="s">
         <v>40</v>
       </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>42</v>
       </c>
-      <c r="G44" t="s">
+      <c r="H44" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45">
         <v>3</v>
       </c>
-      <c r="C45" s="1">
+      <c r="D45" s="1">
         <v>44896.791666666664</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
         <v>16</v>
       </c>
-      <c r="E45" t="s">
+      <c r="F45" t="s">
         <v>43</v>
       </c>
-      <c r="F45" t="s">
+      <c r="G45" t="s">
         <v>39</v>
       </c>
-      <c r="G45" t="s">
+      <c r="H45" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46">
         <v>3</v>
       </c>
-      <c r="C46" s="1">
+      <c r="D46" s="1">
         <v>44897.625</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
         <v>33</v>
       </c>
-      <c r="E46" t="s">
+      <c r="F46" t="s">
         <v>53</v>
       </c>
-      <c r="F46" t="s">
+      <c r="G46" t="s">
         <v>49</v>
       </c>
-      <c r="G46" t="s">
+      <c r="H46" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47">
         <v>3</v>
       </c>
-      <c r="C47" s="1">
+      <c r="D47" s="1">
         <v>44897.625</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
         <v>26</v>
       </c>
-      <c r="E47" t="s">
+      <c r="F47" t="s">
         <v>50</v>
       </c>
-      <c r="F47" t="s">
+      <c r="G47" t="s">
         <v>52</v>
       </c>
-      <c r="G47" t="s">
+      <c r="H47" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48">
         <v>3</v>
       </c>
-      <c r="C48" s="1">
+      <c r="D48" s="1">
         <v>44897.791666666664</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
         <v>30</v>
       </c>
-      <c r="E48" t="s">
+      <c r="F48" t="s">
         <v>55</v>
       </c>
-      <c r="F48" t="s">
+      <c r="G48" t="s">
         <v>46</v>
       </c>
-      <c r="G48" t="s">
+      <c r="H48" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49">
         <v>3</v>
       </c>
-      <c r="C49" s="1">
+      <c r="D49" s="1">
         <v>44897.791666666664</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
         <v>22</v>
       </c>
-      <c r="E49" t="s">
+      <c r="F49" t="s">
         <v>47</v>
       </c>
-      <c r="F49" t="s">
+      <c r="G49" t="s">
         <v>54</v>
       </c>
-      <c r="G49" t="s">
+      <c r="H49" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
         <v>56</v>
       </c>
-      <c r="C50" s="1">
+      <c r="D50" s="1">
         <v>44898.625</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>57</v>
       </c>
-      <c r="E50" t="s">
+      <c r="F50" t="s">
         <v>58</v>
       </c>
-      <c r="F50" t="s">
+      <c r="G50" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" t="s">
         <v>56</v>
       </c>
-      <c r="C51" s="1">
+      <c r="D51" s="1">
         <v>44898.791666666664</v>
       </c>
-      <c r="D51" t="s">
+      <c r="E51" t="s">
         <v>57</v>
       </c>
-      <c r="E51" t="s">
+      <c r="F51" t="s">
         <v>60</v>
       </c>
-      <c r="F51" t="s">
+      <c r="G51" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" t="s">
         <v>56</v>
       </c>
-      <c r="C52" s="1">
+      <c r="D52" s="1">
         <v>44899.791666666664</v>
       </c>
-      <c r="D52" t="s">
+      <c r="E52" t="s">
         <v>57</v>
       </c>
-      <c r="E52" t="s">
+      <c r="F52" t="s">
         <v>64</v>
       </c>
-      <c r="F52" t="s">
+      <c r="G52" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" t="s">
         <v>56</v>
       </c>
-      <c r="C53" s="1">
+      <c r="D53" s="1">
         <v>44899.625</v>
       </c>
-      <c r="D53" t="s">
+      <c r="E53" t="s">
         <v>57</v>
       </c>
-      <c r="E53" t="s">
+      <c r="F53" t="s">
         <v>62</v>
       </c>
-      <c r="F53" t="s">
+      <c r="G53" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" t="s">
         <v>56</v>
       </c>
-      <c r="C54" s="1">
+      <c r="D54" s="1">
         <v>44900.625</v>
       </c>
-      <c r="D54" t="s">
+      <c r="E54" t="s">
         <v>57</v>
       </c>
-      <c r="E54" t="s">
+      <c r="F54" t="s">
         <v>66</v>
       </c>
-      <c r="F54" t="s">
+      <c r="G54" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55" t="s">
         <v>56</v>
       </c>
-      <c r="C55" s="1">
+      <c r="D55" s="1">
         <v>44900.791666666664</v>
       </c>
-      <c r="D55" t="s">
+      <c r="E55" t="s">
         <v>57</v>
       </c>
-      <c r="E55" t="s">
+      <c r="F55" t="s">
         <v>68</v>
       </c>
-      <c r="F55" t="s">
+      <c r="G55" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" t="s">
         <v>56</v>
       </c>
-      <c r="C56" s="1">
+      <c r="D56" s="1">
         <v>44901.625</v>
       </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
         <v>57</v>
       </c>
-      <c r="E56" t="s">
+      <c r="F56" t="s">
         <v>70</v>
       </c>
-      <c r="F56" t="s">
+      <c r="G56" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" t="s">
         <v>56</v>
       </c>
-      <c r="C57" s="1">
+      <c r="D57" s="1">
         <v>44901.791666666664</v>
       </c>
-      <c r="D57" t="s">
+      <c r="E57" t="s">
         <v>57</v>
       </c>
-      <c r="E57" t="s">
+      <c r="F57" t="s">
         <v>72</v>
       </c>
-      <c r="F57" t="s">
+      <c r="G57" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" t="s">
         <v>74</v>
       </c>
-      <c r="C58" s="1">
+      <c r="D58" s="1">
         <v>44904.791666666664</v>
       </c>
-      <c r="D58" t="s">
+      <c r="E58" t="s">
         <v>57</v>
-      </c>
-      <c r="E58" t="s">
-        <v>75</v>
       </c>
       <c r="F58" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G58" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59" t="s">
         <v>74</v>
       </c>
-      <c r="C59" s="1">
+      <c r="D59" s="1">
         <v>44904.625</v>
       </c>
-      <c r="D59" t="s">
+      <c r="E59" t="s">
         <v>57</v>
-      </c>
-      <c r="E59" t="s">
-        <v>75</v>
       </c>
       <c r="F59" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G59" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" t="s">
         <v>74</v>
       </c>
-      <c r="C60" s="1">
+      <c r="D60" s="1">
         <v>44905.791666666664</v>
       </c>
-      <c r="D60" t="s">
+      <c r="E60" t="s">
         <v>57</v>
-      </c>
-      <c r="E60" t="s">
-        <v>75</v>
       </c>
       <c r="F60" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G60" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61" t="s">
         <v>74</v>
       </c>
-      <c r="C61" s="1">
+      <c r="D61" s="1">
         <v>44905.625</v>
       </c>
-      <c r="D61" t="s">
+      <c r="E61" t="s">
         <v>57</v>
-      </c>
-      <c r="E61" t="s">
-        <v>75</v>
       </c>
       <c r="F61" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G61" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62" t="s">
         <v>76</v>
       </c>
-      <c r="C62" s="1">
+      <c r="D62" s="1">
         <v>44908.791666666664</v>
       </c>
-      <c r="D62" t="s">
+      <c r="E62" t="s">
         <v>57</v>
-      </c>
-      <c r="E62" t="s">
-        <v>75</v>
       </c>
       <c r="F62" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G62" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63" t="s">
         <v>76</v>
       </c>
-      <c r="C63" s="1">
+      <c r="D63" s="1">
         <v>44909.791666666664</v>
       </c>
-      <c r="D63" t="s">
+      <c r="E63" t="s">
         <v>57</v>
-      </c>
-      <c r="E63" t="s">
-        <v>75</v>
       </c>
       <c r="F63" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G63" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64" t="s">
         <v>77</v>
       </c>
-      <c r="C64" s="1">
+      <c r="D64" s="1">
         <v>44912.625</v>
       </c>
-      <c r="D64" t="s">
+      <c r="E64" t="s">
         <v>57</v>
-      </c>
-      <c r="E64" t="s">
-        <v>75</v>
       </c>
       <c r="F64" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G64" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65" t="s">
         <v>77</v>
       </c>
-      <c r="C65" s="1">
+      <c r="D65" s="1">
         <v>44913.625</v>
       </c>
-      <c r="D65" t="s">
+      <c r="E65" t="s">
         <v>57</v>
-      </c>
-      <c r="E65" t="s">
-        <v>75</v>
       </c>
       <c r="F65" t="s">
         <v>75</v>
       </c>
+      <c r="G65" t="s">
+        <v>75</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H65">
+  <autoFilter ref="A1:I65" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="7">
+      <filters>
+        <filter val="Group B"/>
+      </filters>
+    </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I65">
       <sortCondition ref="A1:A65"/>
     </sortState>
   </autoFilter>
@@ -2575,184 +2650,211 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:C33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="C1:D33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="2" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C3" t="s">
+    <row r="11" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C4" t="s">
+    <row r="12" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C5" t="s">
+    <row r="13" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C6" t="s">
+    <row r="14" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C7" t="s">
+    <row r="15" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C8" t="s">
+    <row r="16" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C15" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C16" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C26" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C28" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C30" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C31" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C32" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C33" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:C51">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C2:C51">
-      <sortCondition ref="C1:C51"/>
+  <autoFilter ref="C1:D1" xr:uid="{00000000-0001-0000-0100-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C2:D33">
+      <sortCondition ref="D1:D33"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Se concluye la actualización de pertidos y se empieza a trabajar en la base de datos
</commit_message>
<xml_diff>
--- a/docs/fifa-world-cup-2022-UTC_excel.xlsx
+++ b/docs/fifa-world-cup-2022-UTC_excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Documents/PROYECTOS/02.CURSO_HTML/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9547178-0F85-F34F-9492-4877CA9EF5A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F3A9B0F-F94D-6E48-AB71-B7074E5FB67F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="460" windowWidth="12280" windowHeight="17040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1100" yWindow="460" windowWidth="23780" windowHeight="7680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fifa-world-cup-2022-UTC_excel" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'fifa-world-cup-2022-UTC_excel'!$A$1:$I$65</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Hoja1!$C$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Hoja1!$C$1:$D$33</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="113">
   <si>
     <t>Match Number</t>
   </si>
@@ -292,6 +292,78 @@
   </si>
   <si>
     <t>B4</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>G1</t>
+  </si>
+  <si>
+    <t>G2</t>
+  </si>
+  <si>
+    <t>G3</t>
+  </si>
+  <si>
+    <t>G4</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>H3</t>
+  </si>
+  <si>
+    <t>H4</t>
   </si>
 </sst>
 </file>
@@ -1136,13 +1208,13 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -1185,7 +1257,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="1">
-        <v>44886.666666666664</v>
+        <v>44885.666666666664</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
@@ -1226,7 +1298,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1252,7 +1324,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1280,25 +1352,28 @@
     </row>
     <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
+      <c r="C6">
+        <v>13</v>
+      </c>
       <c r="D6" s="1">
-        <v>44887.791666666664</v>
+        <v>44887.416666666664</v>
       </c>
       <c r="E6" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="F6" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="G6" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="H6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -1308,6 +1383,9 @@
       <c r="B7">
         <v>1</v>
       </c>
+      <c r="C7">
+        <v>19</v>
+      </c>
       <c r="D7" s="1">
         <v>44887.541666666664</v>
       </c>
@@ -1331,6 +1409,9 @@
       <c r="B8">
         <v>1</v>
       </c>
+      <c r="C8">
+        <v>14</v>
+      </c>
       <c r="D8" s="1">
         <v>44887.666666666664</v>
       </c>
@@ -1349,45 +1430,51 @@
     </row>
     <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
+      <c r="C9">
+        <v>20</v>
+      </c>
       <c r="D9" s="1">
-        <v>44887.416666666664</v>
+        <v>44887.791666666664</v>
       </c>
       <c r="E9" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="F9" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="G9" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="H9" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
+      <c r="C10">
+        <v>31</v>
+      </c>
       <c r="D10" s="1">
-        <v>44888.791666666664</v>
+        <v>44888.416666666664</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F10" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="G10" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="H10" t="s">
         <v>38</v>
@@ -1395,22 +1482,25 @@
     </row>
     <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
+      <c r="C11">
+        <v>25</v>
+      </c>
       <c r="D11" s="1">
-        <v>44888.666666666664</v>
+        <v>44888.541666666664</v>
       </c>
       <c r="E11" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H11" t="s">
         <v>41</v>
@@ -1418,22 +1508,25 @@
     </row>
     <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
+      <c r="C12">
+        <v>26</v>
+      </c>
       <c r="D12" s="1">
-        <v>44888.541666666664</v>
+        <v>44888.666666666664</v>
       </c>
       <c r="E12" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F12" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G12" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="H12" t="s">
         <v>41</v>
@@ -1441,22 +1534,25 @@
     </row>
     <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
+      <c r="C13">
+        <v>32</v>
+      </c>
       <c r="D13" s="1">
-        <v>44888.416666666664</v>
+        <v>44888.791666666664</v>
       </c>
       <c r="E13" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F13" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="G13" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="H13" t="s">
         <v>38</v>
@@ -1469,6 +1565,9 @@
       <c r="B14">
         <v>1</v>
       </c>
+      <c r="C14">
+        <v>37</v>
+      </c>
       <c r="D14" s="1">
         <v>44889.416666666664</v>
       </c>
@@ -1485,13 +1584,16 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
+      <c r="C15">
+        <v>43</v>
+      </c>
       <c r="D15" s="1">
         <v>44889.541666666664</v>
       </c>
@@ -1508,12 +1610,15 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
         <v>1</v>
+      </c>
+      <c r="C16">
+        <v>44</v>
       </c>
       <c r="D16" s="1">
         <v>44889.666666666664</v>
@@ -1538,6 +1643,9 @@
       <c r="B17">
         <v>1</v>
       </c>
+      <c r="C17">
+        <v>38</v>
+      </c>
       <c r="D17" s="1">
         <v>44889.791666666664</v>
       </c>
@@ -1554,7 +1662,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1632,7 +1740,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1665,6 +1773,9 @@
       <c r="B22">
         <v>2</v>
       </c>
+      <c r="C22">
+        <v>21</v>
+      </c>
       <c r="D22" s="1">
         <v>44891.416666666664</v>
       </c>
@@ -1688,6 +1799,9 @@
       <c r="B23">
         <v>2</v>
       </c>
+      <c r="C23">
+        <v>15</v>
+      </c>
       <c r="D23" s="1">
         <v>44891.541666666664</v>
       </c>
@@ -1711,6 +1825,9 @@
       <c r="B24">
         <v>2</v>
       </c>
+      <c r="C24">
+        <v>22</v>
+      </c>
       <c r="D24" s="1">
         <v>44891.666666666664</v>
       </c>
@@ -1734,6 +1851,9 @@
       <c r="B25">
         <v>2</v>
       </c>
+      <c r="C25">
+        <v>16</v>
+      </c>
       <c r="D25" s="1">
         <v>44891.791666666664</v>
       </c>
@@ -1757,6 +1877,9 @@
       <c r="B26">
         <v>2</v>
       </c>
+      <c r="C26">
+        <v>27</v>
+      </c>
       <c r="D26" s="1">
         <v>44892.416666666664</v>
       </c>
@@ -1780,6 +1903,9 @@
       <c r="B27">
         <v>2</v>
       </c>
+      <c r="C27">
+        <v>33</v>
+      </c>
       <c r="D27" s="1">
         <v>44892.541666666664</v>
       </c>
@@ -1803,6 +1929,9 @@
       <c r="B28">
         <v>2</v>
       </c>
+      <c r="C28">
+        <v>34</v>
+      </c>
       <c r="D28" s="1">
         <v>44892.666666666664</v>
       </c>
@@ -1826,6 +1955,9 @@
       <c r="B29">
         <v>2</v>
       </c>
+      <c r="C29">
+        <v>28</v>
+      </c>
       <c r="D29" s="1">
         <v>44892.791666666664</v>
       </c>
@@ -1849,6 +1981,9 @@
       <c r="B30">
         <v>2</v>
       </c>
+      <c r="C30">
+        <v>39</v>
+      </c>
       <c r="D30" s="1">
         <v>44893.416666666664</v>
       </c>
@@ -1865,12 +2000,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31">
         <v>2</v>
+      </c>
+      <c r="C31">
+        <v>45</v>
       </c>
       <c r="D31" s="1">
         <v>44893.541666666664</v>
@@ -1895,6 +2033,9 @@
       <c r="B32">
         <v>2</v>
       </c>
+      <c r="C32">
+        <v>40</v>
+      </c>
       <c r="D32" s="1">
         <v>44893.666666666664</v>
       </c>
@@ -1911,13 +2052,16 @@
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33">
         <v>2</v>
       </c>
+      <c r="C33">
+        <v>46</v>
+      </c>
       <c r="D33" s="1">
         <v>44893.791666666664</v>
       </c>
@@ -1934,108 +2078,108 @@
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B34">
         <v>3</v>
       </c>
       <c r="C34">
+        <v>5</v>
+      </c>
+      <c r="D34" s="1">
+        <v>44894.625</v>
+      </c>
+      <c r="E34" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" t="s">
+        <v>18</v>
+      </c>
+      <c r="G34" t="s">
+        <v>9</v>
+      </c>
+      <c r="H34" t="s">
         <v>11</v>
       </c>
-      <c r="D34" s="1">
-        <v>44894.791666666664</v>
-      </c>
-      <c r="E34" t="s">
-        <v>19</v>
-      </c>
-      <c r="F34" t="s">
-        <v>21</v>
-      </c>
-      <c r="G34" t="s">
-        <v>13</v>
-      </c>
-      <c r="H34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B35">
         <v>3</v>
       </c>
       <c r="C35">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D35" s="1">
-        <v>44894.791666666664</v>
+        <v>44894.625</v>
       </c>
       <c r="E35" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F35" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G35" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H35" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B36">
         <v>3</v>
       </c>
       <c r="C36">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D36" s="1">
-        <v>44894.625</v>
+        <v>44894.791666666664</v>
       </c>
       <c r="E36" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F36" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G36" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="H36" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B37">
         <v>3</v>
       </c>
       <c r="C37">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D37" s="1">
-        <v>44894.625</v>
+        <v>44894.791666666664</v>
       </c>
       <c r="E37" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F37" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G37" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H37" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
@@ -2045,6 +2189,9 @@
       <c r="B38">
         <v>3</v>
       </c>
+      <c r="C38">
+        <v>23</v>
+      </c>
       <c r="D38" s="1">
         <v>44895.625</v>
       </c>
@@ -2068,6 +2215,9 @@
       <c r="B39">
         <v>3</v>
       </c>
+      <c r="C39">
+        <v>24</v>
+      </c>
       <c r="D39" s="1">
         <v>44895.625</v>
       </c>
@@ -2091,6 +2241,9 @@
       <c r="B40">
         <v>3</v>
       </c>
+      <c r="C40">
+        <v>17</v>
+      </c>
       <c r="D40" s="1">
         <v>44895.791666666664</v>
       </c>
@@ -2114,6 +2267,9 @@
       <c r="B41">
         <v>3</v>
       </c>
+      <c r="C41">
+        <v>18</v>
+      </c>
       <c r="D41" s="1">
         <v>44895.791666666664</v>
       </c>
@@ -2137,6 +2293,9 @@
       <c r="B42">
         <v>3</v>
       </c>
+      <c r="C42">
+        <v>35</v>
+      </c>
       <c r="D42" s="1">
         <v>44896.625</v>
       </c>
@@ -2160,6 +2319,9 @@
       <c r="B43">
         <v>3</v>
       </c>
+      <c r="C43">
+        <v>36</v>
+      </c>
       <c r="D43" s="1">
         <v>44896.625</v>
       </c>
@@ -2183,6 +2345,9 @@
       <c r="B44">
         <v>3</v>
       </c>
+      <c r="C44">
+        <v>29</v>
+      </c>
       <c r="D44" s="1">
         <v>44896.791666666664</v>
       </c>
@@ -2206,6 +2371,9 @@
       <c r="B45">
         <v>3</v>
       </c>
+      <c r="C45">
+        <v>30</v>
+      </c>
       <c r="D45" s="1">
         <v>44896.791666666664</v>
       </c>
@@ -2222,13 +2390,16 @@
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46">
         <v>3</v>
       </c>
+      <c r="C46">
+        <v>47</v>
+      </c>
       <c r="D46" s="1">
         <v>44897.625</v>
       </c>
@@ -2245,12 +2416,15 @@
         <v>51</v>
       </c>
     </row>
-    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47">
         <v>3</v>
+      </c>
+      <c r="C47">
+        <v>48</v>
       </c>
       <c r="D47" s="1">
         <v>44897.625</v>
@@ -2275,6 +2449,9 @@
       <c r="B48">
         <v>3</v>
       </c>
+      <c r="C48">
+        <v>41</v>
+      </c>
       <c r="D48" s="1">
         <v>44897.791666666664</v>
       </c>
@@ -2298,6 +2475,9 @@
       <c r="B49">
         <v>3</v>
       </c>
+      <c r="C49">
+        <v>42</v>
+      </c>
       <c r="D49" s="1">
         <v>44897.791666666664</v>
       </c>
@@ -2356,42 +2536,42 @@
     </row>
     <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B52" t="s">
         <v>56</v>
       </c>
       <c r="D52" s="1">
-        <v>44899.791666666664</v>
+        <v>44899.625</v>
       </c>
       <c r="E52" t="s">
         <v>57</v>
       </c>
       <c r="F52" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G52" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B53" t="s">
         <v>56</v>
       </c>
       <c r="D53" s="1">
-        <v>44899.625</v>
+        <v>44899.791666666664</v>
       </c>
       <c r="E53" t="s">
         <v>57</v>
       </c>
       <c r="F53" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G53" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
@@ -2476,13 +2656,13 @@
     </row>
     <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B58" t="s">
         <v>74</v>
       </c>
       <c r="D58" s="1">
-        <v>44904.791666666664</v>
+        <v>44904.625</v>
       </c>
       <c r="E58" t="s">
         <v>57</v>
@@ -2496,13 +2676,13 @@
     </row>
     <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B59" t="s">
         <v>74</v>
       </c>
       <c r="D59" s="1">
-        <v>44904.625</v>
+        <v>44904.791666666664</v>
       </c>
       <c r="E59" t="s">
         <v>57</v>
@@ -2516,13 +2696,13 @@
     </row>
     <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B60" t="s">
         <v>74</v>
       </c>
       <c r="D60" s="1">
-        <v>44905.791666666664</v>
+        <v>44905.625</v>
       </c>
       <c r="E60" t="s">
         <v>57</v>
@@ -2536,13 +2716,13 @@
     </row>
     <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B61" t="s">
         <v>74</v>
       </c>
       <c r="D61" s="1">
-        <v>44905.625</v>
+        <v>44905.791666666664</v>
       </c>
       <c r="E61" t="s">
         <v>57</v>
@@ -2638,11 +2818,11 @@
   <autoFilter ref="A1:I65" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="7">
       <filters>
-        <filter val="Group B"/>
+        <filter val="Group H"/>
       </filters>
     </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I65">
-      <sortCondition ref="A1:A65"/>
+      <sortCondition ref="D1:D65"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2651,10 +2831,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="C1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2667,7 +2848,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="3:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
         <v>17</v>
       </c>
@@ -2675,7 +2856,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="3:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>18</v>
       </c>
@@ -2683,7 +2864,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="3:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>9</v>
       </c>
@@ -2691,7 +2872,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>10</v>
       </c>
@@ -2699,7 +2880,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>13</v>
       </c>
@@ -2707,7 +2888,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
         <v>14</v>
       </c>
@@ -2715,7 +2896,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
         <v>20</v>
       </c>
@@ -2723,7 +2904,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
         <v>21</v>
       </c>
@@ -2731,129 +2912,204 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="3:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="3:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="3:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="3:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="3:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="3:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="12" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C12" t="s">
+      <c r="D17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="13" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C13" t="s">
+      <c r="D22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="14" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C15" t="s">
+      <c r="D23" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="25" spans="3:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="16" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C19" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C20" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C21" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C22" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C23" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C24" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C25" t="s">
+      <c r="D25" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="3:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C26" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C28" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+      <c r="D28" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="3:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+      <c r="D29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="30" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C30" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="31" spans="3:3" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="D30" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="31" spans="3:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="C31" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="32" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="32" spans="3:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="C32" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="D32" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C33" t="s">
-        <v>49</v>
+        <v>50</v>
+      </c>
+      <c r="D33" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:D1" xr:uid="{00000000-0001-0000-0100-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C2:D33">
+  <autoFilter ref="C1:D33" xr:uid="{00000000-0001-0000-0100-000000000000}">
+    <filterColumn colId="1">
+      <filters blank="1"/>
+    </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C27:D33">
       <sortCondition ref="D1:D33"/>
     </sortState>
   </autoFilter>

</xml_diff>